<commit_message>
Updated to be in sync with current csv files.
</commit_message>
<xml_diff>
--- a/data/_orig/pmhc-upload.xlsx
+++ b/data/_orig/pmhc-upload.xlsx
@@ -825,10 +825,10 @@
         <v>4</v>
       </c>
       <c r="H3">
-        <v>1101</v>
+        <v>1102</v>
       </c>
       <c r="I3">
-        <v>1201</v>
+        <v>1202</v>
       </c>
       <c r="J3">
         <v>3</v>
@@ -848,7 +848,7 @@
         <v>28021983</v>
       </c>
       <c r="E4">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F4">
         <v>2</v>
@@ -873,13 +873,13 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:AA3"/>
+  <dimension ref="A1:Z3"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:27">
+    <row r="1" spans="1:26">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -887,7 +887,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:27">
+    <row r="2" spans="1:26">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -967,7 +967,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="3" spans="1:27">
+    <row r="3" spans="1:26">
       <c r="A3" t="s">
         <v>39</v>
       </c>
@@ -990,7 +990,7 @@
         <v>12022016</v>
       </c>
       <c r="H3">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="I3">
         <v>3</v>
@@ -1044,9 +1044,6 @@
         <v>2</v>
       </c>
       <c r="Z3">
-        <v>1</v>
-      </c>
-      <c r="AA3">
         <v>1</v>
       </c>
     </row>
@@ -1486,7 +1483,7 @@
         <v>18062016</v>
       </c>
       <c r="E3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F3">
         <v>1</v>
@@ -1904,7 +1901,7 @@
         <v>56</v>
       </c>
       <c r="C3">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="D3">
         <v>1</v>

</xml_diff>

<commit_message>
Added tags field to each record type.
</commit_message>
<xml_diff>
--- a/data/_orig/pmhc-upload.xlsx
+++ b/data/_orig/pmhc-upload.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="183" uniqueCount="135">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="199" uniqueCount="147">
   <si>
     <t>Version</t>
   </si>
@@ -55,7 +55,10 @@
     <t>prof_english</t>
   </si>
   <si>
-    <t>PHN_01:Test PHN</t>
+    <t>client_tags</t>
+  </si>
+  <si>
+    <t>PHN999:NFP01</t>
   </si>
   <si>
     <t>CL01</t>
@@ -64,6 +67,9 @@
     <t>ee12371ef32e847f3ea6a36adcb0050bfbc2ff84</t>
   </si>
   <si>
+    <t>tag1 tag3</t>
+  </si>
+  <si>
     <t>CL02</t>
   </si>
   <si>
@@ -76,6 +82,9 @@
     <t>episode_end_date</t>
   </si>
   <si>
+    <t>client_consent</t>
+  </si>
+  <si>
     <t>episode_completion_status</t>
   </si>
   <si>
@@ -85,6 +94,9 @@
     <t>principal_focus</t>
   </si>
   <si>
+    <t>mental_health_treatment_plan</t>
+  </si>
+  <si>
     <t>homelessness</t>
   </si>
   <si>
@@ -139,12 +151,15 @@
     <t>referrer_organisation_type</t>
   </si>
   <si>
-    <t>PHN01:PO01</t>
+    <t>episode_tags</t>
   </si>
   <si>
     <t>E01</t>
   </si>
   <si>
+    <t>tag3</t>
+  </si>
+  <si>
     <t>service_contact_key</t>
   </si>
   <si>
@@ -187,6 +202,9 @@
     <t>service_contact_final</t>
   </si>
   <si>
+    <t>service_contact_tags</t>
+  </si>
+  <si>
     <t>SC01</t>
   </si>
   <si>
@@ -196,6 +214,9 @@
     <t>SC02</t>
   </si>
   <si>
+    <t>tag1</t>
+  </si>
+  <si>
     <t>collection_occasion_key</t>
   </si>
   <si>
@@ -247,6 +268,9 @@
     <t>k10p_item14</t>
   </si>
   <si>
+    <t>k10p_tags</t>
+  </si>
+  <si>
     <t>CO01</t>
   </si>
   <si>
@@ -268,6 +292,12 @@
     <t>k5_item5</t>
   </si>
   <si>
+    <t>k5_tags</t>
+  </si>
+  <si>
+    <t>tag1 tag2</t>
+  </si>
+  <si>
     <t>sdq_version</t>
   </si>
   <si>
@@ -397,6 +427,9 @@
     <t>sdq_item42</t>
   </si>
   <si>
+    <t>sdq_tags</t>
+  </si>
+  <si>
     <t>PC101</t>
   </si>
   <si>
@@ -418,10 +451,13 @@
     <t>practitioner_active</t>
   </si>
   <si>
-    <t>PHC01:PO01</t>
+    <t>practitioner_tags</t>
   </si>
   <si>
     <t>P02</t>
+  </si>
+  <si>
+    <t>tag2 tag3</t>
   </si>
   <si>
     <t>P03</t>
@@ -756,13 +792,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:J4"/>
+  <dimension ref="A1:K4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:10">
+    <row r="1" spans="1:11">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -770,7 +806,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:10">
+    <row r="2" spans="1:11">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -801,16 +837,19 @@
       <c r="J2" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="3" spans="1:10">
+      <c r="K2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11">
       <c r="A3" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B3" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C3" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="D3">
         <v>28021983</v>
@@ -833,16 +872,19 @@
       <c r="J3">
         <v>3</v>
       </c>
-    </row>
-    <row r="4" spans="1:10">
+      <c r="K3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11">
       <c r="A4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B4" t="s">
+        <v>16</v>
+      </c>
+      <c r="C4" t="s">
         <v>14</v>
-      </c>
-      <c r="C4" t="s">
-        <v>13</v>
       </c>
       <c r="D4">
         <v>28021983</v>
@@ -873,13 +915,13 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:Z3"/>
+  <dimension ref="A1:AC3"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:26">
+    <row r="1" spans="1:29">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -887,95 +929,104 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:26">
+    <row r="2" spans="1:29">
       <c r="A2" t="s">
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="C2" t="s">
         <v>2</v>
       </c>
       <c r="D2" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="E2" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="F2" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="G2" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="H2" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="I2" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="J2" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="K2" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="L2" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="M2" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="N2" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="O2" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="P2" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="Q2" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="R2" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="S2" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="T2" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="U2" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="V2" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="W2" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="X2" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="Y2" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="Z2" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="3" spans="1:26">
+        <v>40</v>
+      </c>
+      <c r="AA2" t="s">
+        <v>41</v>
+      </c>
+      <c r="AB2" t="s">
+        <v>42</v>
+      </c>
+      <c r="AC2" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="3" spans="1:29">
       <c r="A3" t="s">
-        <v>39</v>
+        <v>12</v>
       </c>
       <c r="B3" t="s">
-        <v>40</v>
+        <v>44</v>
       </c>
       <c r="C3" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D3">
         <v>13032016</v>
@@ -987,50 +1038,50 @@
         <v>1</v>
       </c>
       <c r="G3">
+        <v>1</v>
+      </c>
+      <c r="H3">
         <v>12022016</v>
       </c>
-      <c r="H3">
-        <v>2</v>
-      </c>
       <c r="I3">
+        <v>2</v>
+      </c>
+      <c r="J3">
         <v>3</v>
       </c>
-      <c r="J3">
+      <c r="K3">
+        <v>1</v>
+      </c>
+      <c r="L3">
         <v>1101</v>
       </c>
-      <c r="K3">
-        <v>1</v>
-      </c>
-      <c r="L3">
-        <v>1</v>
-      </c>
       <c r="M3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="N3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="O3">
         <v>2</v>
       </c>
       <c r="P3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="Q3">
         <v>2</v>
       </c>
       <c r="R3">
+        <v>1</v>
+      </c>
+      <c r="S3">
+        <v>2</v>
+      </c>
+      <c r="T3">
         <v>107</v>
       </c>
-      <c r="S3">
+      <c r="U3">
         <v>903</v>
       </c>
-      <c r="T3">
-        <v>2</v>
-      </c>
-      <c r="U3">
-        <v>2</v>
-      </c>
       <c r="V3">
         <v>2</v>
       </c>
@@ -1044,7 +1095,16 @@
         <v>2</v>
       </c>
       <c r="Z3">
-        <v>1</v>
+        <v>2</v>
+      </c>
+      <c r="AA3">
+        <v>2</v>
+      </c>
+      <c r="AB3">
+        <v>1</v>
+      </c>
+      <c r="AC3" t="s">
+        <v>45</v>
       </c>
     </row>
   </sheetData>
@@ -1054,13 +1114,13 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:P4"/>
+  <dimension ref="A1:Q4"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:16">
+    <row r="1" spans="1:17">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1068,68 +1128,71 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:16">
+    <row r="2" spans="1:17">
       <c r="A2" t="s">
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
       <c r="C2" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="D2" t="s">
-        <v>42</v>
+        <v>47</v>
       </c>
       <c r="E2" t="s">
-        <v>43</v>
+        <v>48</v>
       </c>
       <c r="F2" t="s">
+        <v>49</v>
+      </c>
+      <c r="G2" t="s">
+        <v>50</v>
+      </c>
+      <c r="H2" t="s">
+        <v>51</v>
+      </c>
+      <c r="I2" t="s">
+        <v>52</v>
+      </c>
+      <c r="J2" t="s">
+        <v>53</v>
+      </c>
+      <c r="K2" t="s">
+        <v>54</v>
+      </c>
+      <c r="L2" t="s">
+        <v>55</v>
+      </c>
+      <c r="M2" t="s">
+        <v>56</v>
+      </c>
+      <c r="N2" t="s">
+        <v>57</v>
+      </c>
+      <c r="O2" t="s">
+        <v>58</v>
+      </c>
+      <c r="P2" t="s">
+        <v>59</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17">
+      <c r="A3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B3" t="s">
+        <v>61</v>
+      </c>
+      <c r="C3" t="s">
         <v>44</v>
       </c>
-      <c r="G2" t="s">
-        <v>45</v>
-      </c>
-      <c r="H2" t="s">
-        <v>46</v>
-      </c>
-      <c r="I2" t="s">
-        <v>47</v>
-      </c>
-      <c r="J2" t="s">
-        <v>48</v>
-      </c>
-      <c r="K2" t="s">
-        <v>49</v>
-      </c>
-      <c r="L2" t="s">
-        <v>50</v>
-      </c>
-      <c r="M2" t="s">
-        <v>51</v>
-      </c>
-      <c r="N2" t="s">
-        <v>52</v>
-      </c>
-      <c r="O2" t="s">
-        <v>53</v>
-      </c>
-      <c r="P2" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="3" spans="1:16">
-      <c r="A3" t="s">
-        <v>39</v>
-      </c>
-      <c r="B3" t="s">
-        <v>55</v>
-      </c>
-      <c r="C3" t="s">
-        <v>40</v>
-      </c>
       <c r="D3" t="s">
-        <v>56</v>
+        <v>62</v>
       </c>
       <c r="E3">
         <v>18062016</v>
@@ -1168,18 +1231,18 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:16">
+    <row r="4" spans="1:17">
       <c r="A4" t="s">
-        <v>39</v>
+        <v>12</v>
       </c>
       <c r="B4" t="s">
-        <v>57</v>
+        <v>63</v>
       </c>
       <c r="C4" t="s">
-        <v>40</v>
+        <v>44</v>
       </c>
       <c r="D4" t="s">
-        <v>56</v>
+        <v>62</v>
       </c>
       <c r="E4">
         <v>18062016</v>
@@ -1216,6 +1279,9 @@
       </c>
       <c r="P4">
         <v>3</v>
+      </c>
+      <c r="Q4" t="s">
+        <v>64</v>
       </c>
     </row>
   </sheetData>
@@ -1225,13 +1291,13 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:S4"/>
+  <dimension ref="A1:T4"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:19">
+    <row r="1" spans="1:20">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1239,74 +1305,77 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:19">
+    <row r="2" spans="1:20">
       <c r="A2" t="s">
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>58</v>
+        <v>65</v>
       </c>
       <c r="C2" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="D2" t="s">
-        <v>59</v>
+        <v>66</v>
       </c>
       <c r="E2" t="s">
-        <v>60</v>
+        <v>67</v>
       </c>
       <c r="F2" t="s">
-        <v>61</v>
+        <v>68</v>
       </c>
       <c r="G2" t="s">
-        <v>62</v>
+        <v>69</v>
       </c>
       <c r="H2" t="s">
-        <v>63</v>
+        <v>70</v>
       </c>
       <c r="I2" t="s">
-        <v>64</v>
+        <v>71</v>
       </c>
       <c r="J2" t="s">
-        <v>65</v>
+        <v>72</v>
       </c>
       <c r="K2" t="s">
-        <v>66</v>
+        <v>73</v>
       </c>
       <c r="L2" t="s">
-        <v>67</v>
+        <v>74</v>
       </c>
       <c r="M2" t="s">
-        <v>68</v>
+        <v>75</v>
       </c>
       <c r="N2" t="s">
-        <v>69</v>
+        <v>76</v>
       </c>
       <c r="O2" t="s">
-        <v>70</v>
+        <v>77</v>
       </c>
       <c r="P2" t="s">
-        <v>71</v>
+        <v>78</v>
       </c>
       <c r="Q2" t="s">
-        <v>72</v>
+        <v>79</v>
       </c>
       <c r="R2" t="s">
-        <v>73</v>
+        <v>80</v>
       </c>
       <c r="S2" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="3" spans="1:19">
+        <v>81</v>
+      </c>
+      <c r="T2" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="3" spans="1:20">
       <c r="A3" t="s">
-        <v>39</v>
+        <v>12</v>
       </c>
       <c r="B3" t="s">
-        <v>75</v>
+        <v>83</v>
       </c>
       <c r="C3" t="s">
-        <v>40</v>
+        <v>44</v>
       </c>
       <c r="D3">
         <v>18062016</v>
@@ -1357,15 +1426,15 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:19">
+    <row r="4" spans="1:20">
       <c r="A4" t="s">
-        <v>39</v>
+        <v>12</v>
       </c>
       <c r="B4" t="s">
-        <v>76</v>
+        <v>84</v>
       </c>
       <c r="C4" t="s">
-        <v>40</v>
+        <v>44</v>
       </c>
       <c r="D4">
         <v>18062016</v>
@@ -1414,6 +1483,9 @@
       </c>
       <c r="S4">
         <v>3</v>
+      </c>
+      <c r="T4" t="s">
+        <v>64</v>
       </c>
     </row>
   </sheetData>
@@ -1423,13 +1495,13 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:J4"/>
+  <dimension ref="A1:K4"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:10">
+    <row r="1" spans="1:11">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1437,47 +1509,50 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:10">
+    <row r="2" spans="1:11">
       <c r="A2" t="s">
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>58</v>
+        <v>65</v>
       </c>
       <c r="C2" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="D2" t="s">
-        <v>59</v>
+        <v>66</v>
       </c>
       <c r="E2" t="s">
-        <v>60</v>
+        <v>67</v>
       </c>
       <c r="F2" t="s">
-        <v>77</v>
+        <v>85</v>
       </c>
       <c r="G2" t="s">
-        <v>78</v>
+        <v>86</v>
       </c>
       <c r="H2" t="s">
-        <v>79</v>
+        <v>87</v>
       </c>
       <c r="I2" t="s">
-        <v>80</v>
+        <v>88</v>
       </c>
       <c r="J2" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10">
+        <v>89</v>
+      </c>
+      <c r="K2" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11">
       <c r="A3" t="s">
-        <v>39</v>
+        <v>12</v>
       </c>
       <c r="B3" t="s">
-        <v>75</v>
+        <v>83</v>
       </c>
       <c r="C3" t="s">
-        <v>40</v>
+        <v>44</v>
       </c>
       <c r="D3">
         <v>18062016</v>
@@ -1500,16 +1575,19 @@
       <c r="J3">
         <v>5</v>
       </c>
-    </row>
-    <row r="4" spans="1:10">
+      <c r="K3" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11">
       <c r="A4" t="s">
-        <v>39</v>
+        <v>12</v>
       </c>
       <c r="B4" t="s">
-        <v>76</v>
+        <v>84</v>
       </c>
       <c r="C4" t="s">
-        <v>40</v>
+        <v>44</v>
       </c>
       <c r="D4">
         <v>18062016</v>
@@ -1540,13 +1618,13 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:AV3"/>
+  <dimension ref="A1:AW3"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:48">
+    <row r="1" spans="1:49">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1554,161 +1632,164 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:48">
+    <row r="2" spans="1:49">
       <c r="A2" t="s">
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>58</v>
+        <v>65</v>
       </c>
       <c r="C2" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="D2" t="s">
-        <v>59</v>
+        <v>66</v>
       </c>
       <c r="E2" t="s">
-        <v>60</v>
+        <v>67</v>
       </c>
       <c r="F2" t="s">
-        <v>82</v>
+        <v>92</v>
       </c>
       <c r="G2" t="s">
+        <v>93</v>
+      </c>
+      <c r="H2" t="s">
+        <v>94</v>
+      </c>
+      <c r="I2" t="s">
+        <v>95</v>
+      </c>
+      <c r="J2" t="s">
+        <v>96</v>
+      </c>
+      <c r="K2" t="s">
+        <v>97</v>
+      </c>
+      <c r="L2" t="s">
+        <v>98</v>
+      </c>
+      <c r="M2" t="s">
+        <v>99</v>
+      </c>
+      <c r="N2" t="s">
+        <v>100</v>
+      </c>
+      <c r="O2" t="s">
+        <v>101</v>
+      </c>
+      <c r="P2" t="s">
+        <v>102</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>103</v>
+      </c>
+      <c r="R2" t="s">
+        <v>104</v>
+      </c>
+      <c r="S2" t="s">
+        <v>105</v>
+      </c>
+      <c r="T2" t="s">
+        <v>106</v>
+      </c>
+      <c r="U2" t="s">
+        <v>107</v>
+      </c>
+      <c r="V2" t="s">
+        <v>108</v>
+      </c>
+      <c r="W2" t="s">
+        <v>109</v>
+      </c>
+      <c r="X2" t="s">
+        <v>110</v>
+      </c>
+      <c r="Y2" t="s">
+        <v>111</v>
+      </c>
+      <c r="Z2" t="s">
+        <v>112</v>
+      </c>
+      <c r="AA2" t="s">
+        <v>113</v>
+      </c>
+      <c r="AB2" t="s">
+        <v>114</v>
+      </c>
+      <c r="AC2" t="s">
+        <v>115</v>
+      </c>
+      <c r="AD2" t="s">
+        <v>116</v>
+      </c>
+      <c r="AE2" t="s">
+        <v>117</v>
+      </c>
+      <c r="AF2" t="s">
+        <v>118</v>
+      </c>
+      <c r="AG2" t="s">
+        <v>119</v>
+      </c>
+      <c r="AH2" t="s">
+        <v>120</v>
+      </c>
+      <c r="AI2" t="s">
+        <v>121</v>
+      </c>
+      <c r="AJ2" t="s">
+        <v>122</v>
+      </c>
+      <c r="AK2" t="s">
+        <v>123</v>
+      </c>
+      <c r="AL2" t="s">
+        <v>124</v>
+      </c>
+      <c r="AM2" t="s">
+        <v>125</v>
+      </c>
+      <c r="AN2" t="s">
+        <v>126</v>
+      </c>
+      <c r="AO2" t="s">
+        <v>127</v>
+      </c>
+      <c r="AP2" t="s">
+        <v>128</v>
+      </c>
+      <c r="AQ2" t="s">
+        <v>129</v>
+      </c>
+      <c r="AR2" t="s">
+        <v>130</v>
+      </c>
+      <c r="AS2" t="s">
+        <v>131</v>
+      </c>
+      <c r="AT2" t="s">
+        <v>132</v>
+      </c>
+      <c r="AU2" t="s">
+        <v>133</v>
+      </c>
+      <c r="AV2" t="s">
+        <v>134</v>
+      </c>
+      <c r="AW2" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="3" spans="1:49">
+      <c r="A3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B3" t="s">
         <v>83</v>
       </c>
-      <c r="H2" t="s">
-        <v>84</v>
-      </c>
-      <c r="I2" t="s">
-        <v>85</v>
-      </c>
-      <c r="J2" t="s">
-        <v>86</v>
-      </c>
-      <c r="K2" t="s">
-        <v>87</v>
-      </c>
-      <c r="L2" t="s">
-        <v>88</v>
-      </c>
-      <c r="M2" t="s">
-        <v>89</v>
-      </c>
-      <c r="N2" t="s">
-        <v>90</v>
-      </c>
-      <c r="O2" t="s">
-        <v>91</v>
-      </c>
-      <c r="P2" t="s">
-        <v>92</v>
-      </c>
-      <c r="Q2" t="s">
-        <v>93</v>
-      </c>
-      <c r="R2" t="s">
-        <v>94</v>
-      </c>
-      <c r="S2" t="s">
-        <v>95</v>
-      </c>
-      <c r="T2" t="s">
-        <v>96</v>
-      </c>
-      <c r="U2" t="s">
-        <v>97</v>
-      </c>
-      <c r="V2" t="s">
-        <v>98</v>
-      </c>
-      <c r="W2" t="s">
-        <v>99</v>
-      </c>
-      <c r="X2" t="s">
-        <v>100</v>
-      </c>
-      <c r="Y2" t="s">
-        <v>101</v>
-      </c>
-      <c r="Z2" t="s">
-        <v>102</v>
-      </c>
-      <c r="AA2" t="s">
-        <v>103</v>
-      </c>
-      <c r="AB2" t="s">
-        <v>104</v>
-      </c>
-      <c r="AC2" t="s">
-        <v>105</v>
-      </c>
-      <c r="AD2" t="s">
-        <v>106</v>
-      </c>
-      <c r="AE2" t="s">
-        <v>107</v>
-      </c>
-      <c r="AF2" t="s">
-        <v>108</v>
-      </c>
-      <c r="AG2" t="s">
-        <v>109</v>
-      </c>
-      <c r="AH2" t="s">
-        <v>110</v>
-      </c>
-      <c r="AI2" t="s">
-        <v>111</v>
-      </c>
-      <c r="AJ2" t="s">
-        <v>112</v>
-      </c>
-      <c r="AK2" t="s">
-        <v>113</v>
-      </c>
-      <c r="AL2" t="s">
-        <v>114</v>
-      </c>
-      <c r="AM2" t="s">
-        <v>115</v>
-      </c>
-      <c r="AN2" t="s">
-        <v>116</v>
-      </c>
-      <c r="AO2" t="s">
-        <v>117</v>
-      </c>
-      <c r="AP2" t="s">
-        <v>118</v>
-      </c>
-      <c r="AQ2" t="s">
-        <v>119</v>
-      </c>
-      <c r="AR2" t="s">
-        <v>120</v>
-      </c>
-      <c r="AS2" t="s">
-        <v>121</v>
-      </c>
-      <c r="AT2" t="s">
-        <v>122</v>
-      </c>
-      <c r="AU2" t="s">
-        <v>123</v>
-      </c>
-      <c r="AV2" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="3" spans="1:48">
-      <c r="A3" t="s">
-        <v>39</v>
-      </c>
-      <c r="B3" t="s">
-        <v>75</v>
-      </c>
       <c r="C3" t="s">
-        <v>40</v>
+        <v>44</v>
       </c>
       <c r="D3">
         <v>16062016</v>
@@ -1717,7 +1798,7 @@
         <v>1</v>
       </c>
       <c r="F3" t="s">
-        <v>125</v>
+        <v>136</v>
       </c>
       <c r="G3">
         <v>2</v>
@@ -1853,13 +1934,13 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H5"/>
+  <dimension ref="A1:I5"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:8">
+    <row r="1" spans="1:9">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1867,38 +1948,41 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:8">
+    <row r="2" spans="1:9">
       <c r="A2" t="s">
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>42</v>
+        <v>47</v>
       </c>
       <c r="C2" t="s">
-        <v>126</v>
+        <v>137</v>
       </c>
       <c r="D2" t="s">
-        <v>127</v>
+        <v>138</v>
       </c>
       <c r="E2" t="s">
-        <v>128</v>
+        <v>139</v>
       </c>
       <c r="F2" t="s">
-        <v>129</v>
+        <v>140</v>
       </c>
       <c r="G2" t="s">
-        <v>130</v>
+        <v>141</v>
       </c>
       <c r="H2" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8">
+        <v>142</v>
+      </c>
+      <c r="I2" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9">
       <c r="A3" t="s">
-        <v>132</v>
+        <v>12</v>
       </c>
       <c r="B3" t="s">
-        <v>56</v>
+        <v>62</v>
       </c>
       <c r="C3">
         <v>8</v>
@@ -1918,13 +2002,16 @@
       <c r="H3">
         <v>1</v>
       </c>
-    </row>
-    <row r="4" spans="1:8">
+      <c r="I3" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9">
       <c r="A4" t="s">
-        <v>132</v>
+        <v>12</v>
       </c>
       <c r="B4" t="s">
-        <v>133</v>
+        <v>144</v>
       </c>
       <c r="C4">
         <v>2</v>
@@ -1941,13 +2028,16 @@
       <c r="H4">
         <v>1</v>
       </c>
-    </row>
-    <row r="5" spans="1:8">
+      <c r="I4" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9">
       <c r="A5" t="s">
-        <v>132</v>
+        <v>12</v>
       </c>
       <c r="B5" t="s">
-        <v>134</v>
+        <v>146</v>
       </c>
       <c r="C5">
         <v>2</v>

</xml_diff>

<commit_message>
Removed episode_start_date as it is a derived field. Updated domain of episode_completion_status
</commit_message>
<xml_diff>
--- a/data/_orig/pmhc-upload.xlsx
+++ b/data/_orig/pmhc-upload.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="199" uniqueCount="147">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="198" uniqueCount="146">
   <si>
     <t>Version</t>
   </si>
@@ -74,9 +74,6 @@
   </si>
   <si>
     <t>episode_key</t>
-  </si>
-  <si>
-    <t>episode_start_date</t>
   </si>
   <si>
     <t>episode_end_date</t>
@@ -915,13 +912,13 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:AC3"/>
+  <dimension ref="A1:AB3"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:29">
+    <row r="1" spans="1:28">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -929,7 +926,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:29">
+    <row r="2" spans="1:28">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -1014,52 +1011,49 @@
       <c r="AB2" t="s">
         <v>42</v>
       </c>
-      <c r="AC2" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="3" spans="1:29">
+    </row>
+    <row r="3" spans="1:28">
       <c r="A3" t="s">
         <v>12</v>
       </c>
       <c r="B3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C3" t="s">
         <v>13</v>
       </c>
       <c r="D3">
-        <v>13032016</v>
+        <v>18062016</v>
       </c>
       <c r="E3">
-        <v>18062016</v>
+        <v>1</v>
       </c>
       <c r="F3">
         <v>1</v>
       </c>
       <c r="G3">
-        <v>1</v>
+        <v>12022016</v>
       </c>
       <c r="H3">
-        <v>12022016</v>
+        <v>2</v>
       </c>
       <c r="I3">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="J3">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="K3">
-        <v>1</v>
+        <v>1101</v>
       </c>
       <c r="L3">
-        <v>1101</v>
+        <v>1</v>
       </c>
       <c r="M3">
         <v>1</v>
       </c>
       <c r="N3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="O3">
         <v>2</v>
@@ -1068,19 +1062,19 @@
         <v>2</v>
       </c>
       <c r="Q3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="R3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="S3">
-        <v>2</v>
+        <v>107</v>
       </c>
       <c r="T3">
-        <v>107</v>
+        <v>903</v>
       </c>
       <c r="U3">
-        <v>903</v>
+        <v>2</v>
       </c>
       <c r="V3">
         <v>2</v>
@@ -1098,13 +1092,10 @@
         <v>2</v>
       </c>
       <c r="AA3">
-        <v>2</v>
-      </c>
-      <c r="AB3">
-        <v>1</v>
-      </c>
-      <c r="AC3" t="s">
-        <v>45</v>
+        <v>1</v>
+      </c>
+      <c r="AB3" t="s">
+        <v>44</v>
       </c>
     </row>
   </sheetData>
@@ -1133,52 +1124,52 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C2" t="s">
         <v>17</v>
       </c>
       <c r="D2" t="s">
+        <v>46</v>
+      </c>
+      <c r="E2" t="s">
         <v>47</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F2" t="s">
         <v>48</v>
       </c>
-      <c r="F2" t="s">
+      <c r="G2" t="s">
         <v>49</v>
       </c>
-      <c r="G2" t="s">
+      <c r="H2" t="s">
         <v>50</v>
       </c>
-      <c r="H2" t="s">
+      <c r="I2" t="s">
         <v>51</v>
       </c>
-      <c r="I2" t="s">
+      <c r="J2" t="s">
         <v>52</v>
       </c>
-      <c r="J2" t="s">
+      <c r="K2" t="s">
         <v>53</v>
       </c>
-      <c r="K2" t="s">
+      <c r="L2" t="s">
         <v>54</v>
       </c>
-      <c r="L2" t="s">
+      <c r="M2" t="s">
         <v>55</v>
       </c>
-      <c r="M2" t="s">
+      <c r="N2" t="s">
         <v>56</v>
       </c>
-      <c r="N2" t="s">
+      <c r="O2" t="s">
         <v>57</v>
       </c>
-      <c r="O2" t="s">
+      <c r="P2" t="s">
         <v>58</v>
       </c>
-      <c r="P2" t="s">
+      <c r="Q2" t="s">
         <v>59</v>
-      </c>
-      <c r="Q2" t="s">
-        <v>60</v>
       </c>
     </row>
     <row r="3" spans="1:17">
@@ -1186,13 +1177,13 @@
         <v>12</v>
       </c>
       <c r="B3" t="s">
+        <v>60</v>
+      </c>
+      <c r="C3" t="s">
+        <v>43</v>
+      </c>
+      <c r="D3" t="s">
         <v>61</v>
-      </c>
-      <c r="C3" t="s">
-        <v>44</v>
-      </c>
-      <c r="D3" t="s">
-        <v>62</v>
       </c>
       <c r="E3">
         <v>18062016</v>
@@ -1236,13 +1227,13 @@
         <v>12</v>
       </c>
       <c r="B4" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C4" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D4" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E4">
         <v>18062016</v>
@@ -1281,7 +1272,7 @@
         <v>3</v>
       </c>
       <c r="Q4" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
   </sheetData>
@@ -1310,61 +1301,61 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C2" t="s">
         <v>17</v>
       </c>
       <c r="D2" t="s">
+        <v>65</v>
+      </c>
+      <c r="E2" t="s">
         <v>66</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F2" t="s">
         <v>67</v>
       </c>
-      <c r="F2" t="s">
+      <c r="G2" t="s">
         <v>68</v>
       </c>
-      <c r="G2" t="s">
+      <c r="H2" t="s">
         <v>69</v>
       </c>
-      <c r="H2" t="s">
+      <c r="I2" t="s">
         <v>70</v>
       </c>
-      <c r="I2" t="s">
+      <c r="J2" t="s">
         <v>71</v>
       </c>
-      <c r="J2" t="s">
+      <c r="K2" t="s">
         <v>72</v>
       </c>
-      <c r="K2" t="s">
+      <c r="L2" t="s">
         <v>73</v>
       </c>
-      <c r="L2" t="s">
+      <c r="M2" t="s">
         <v>74</v>
       </c>
-      <c r="M2" t="s">
+      <c r="N2" t="s">
         <v>75</v>
       </c>
-      <c r="N2" t="s">
+      <c r="O2" t="s">
         <v>76</v>
       </c>
-      <c r="O2" t="s">
+      <c r="P2" t="s">
         <v>77</v>
       </c>
-      <c r="P2" t="s">
+      <c r="Q2" t="s">
         <v>78</v>
       </c>
-      <c r="Q2" t="s">
+      <c r="R2" t="s">
         <v>79</v>
       </c>
-      <c r="R2" t="s">
+      <c r="S2" t="s">
         <v>80</v>
       </c>
-      <c r="S2" t="s">
+      <c r="T2" t="s">
         <v>81</v>
-      </c>
-      <c r="T2" t="s">
-        <v>82</v>
       </c>
     </row>
     <row r="3" spans="1:20">
@@ -1372,10 +1363,10 @@
         <v>12</v>
       </c>
       <c r="B3" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D3">
         <v>18062016</v>
@@ -1431,10 +1422,10 @@
         <v>12</v>
       </c>
       <c r="B4" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C4" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D4">
         <v>18062016</v>
@@ -1485,7 +1476,7 @@
         <v>3</v>
       </c>
       <c r="T4" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
   </sheetData>
@@ -1514,34 +1505,34 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C2" t="s">
         <v>17</v>
       </c>
       <c r="D2" t="s">
+        <v>65</v>
+      </c>
+      <c r="E2" t="s">
         <v>66</v>
       </c>
-      <c r="E2" t="s">
-        <v>67</v>
-      </c>
       <c r="F2" t="s">
+        <v>84</v>
+      </c>
+      <c r="G2" t="s">
         <v>85</v>
       </c>
-      <c r="G2" t="s">
+      <c r="H2" t="s">
         <v>86</v>
       </c>
-      <c r="H2" t="s">
+      <c r="I2" t="s">
         <v>87</v>
       </c>
-      <c r="I2" t="s">
+      <c r="J2" t="s">
         <v>88</v>
       </c>
-      <c r="J2" t="s">
+      <c r="K2" t="s">
         <v>89</v>
-      </c>
-      <c r="K2" t="s">
-        <v>90</v>
       </c>
     </row>
     <row r="3" spans="1:11">
@@ -1549,10 +1540,10 @@
         <v>12</v>
       </c>
       <c r="B3" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D3">
         <v>18062016</v>
@@ -1576,7 +1567,7 @@
         <v>5</v>
       </c>
       <c r="K3" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="4" spans="1:11">
@@ -1584,10 +1575,10 @@
         <v>12</v>
       </c>
       <c r="B4" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C4" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D4">
         <v>18062016</v>
@@ -1637,148 +1628,148 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C2" t="s">
         <v>17</v>
       </c>
       <c r="D2" t="s">
+        <v>65</v>
+      </c>
+      <c r="E2" t="s">
         <v>66</v>
       </c>
-      <c r="E2" t="s">
-        <v>67</v>
-      </c>
       <c r="F2" t="s">
+        <v>91</v>
+      </c>
+      <c r="G2" t="s">
         <v>92</v>
       </c>
-      <c r="G2" t="s">
+      <c r="H2" t="s">
         <v>93</v>
       </c>
-      <c r="H2" t="s">
+      <c r="I2" t="s">
         <v>94</v>
       </c>
-      <c r="I2" t="s">
+      <c r="J2" t="s">
         <v>95</v>
       </c>
-      <c r="J2" t="s">
+      <c r="K2" t="s">
         <v>96</v>
       </c>
-      <c r="K2" t="s">
+      <c r="L2" t="s">
         <v>97</v>
       </c>
-      <c r="L2" t="s">
+      <c r="M2" t="s">
         <v>98</v>
       </c>
-      <c r="M2" t="s">
+      <c r="N2" t="s">
         <v>99</v>
       </c>
-      <c r="N2" t="s">
+      <c r="O2" t="s">
         <v>100</v>
       </c>
-      <c r="O2" t="s">
+      <c r="P2" t="s">
         <v>101</v>
       </c>
-      <c r="P2" t="s">
+      <c r="Q2" t="s">
         <v>102</v>
       </c>
-      <c r="Q2" t="s">
+      <c r="R2" t="s">
         <v>103</v>
       </c>
-      <c r="R2" t="s">
+      <c r="S2" t="s">
         <v>104</v>
       </c>
-      <c r="S2" t="s">
+      <c r="T2" t="s">
         <v>105</v>
       </c>
-      <c r="T2" t="s">
+      <c r="U2" t="s">
         <v>106</v>
       </c>
-      <c r="U2" t="s">
+      <c r="V2" t="s">
         <v>107</v>
       </c>
-      <c r="V2" t="s">
+      <c r="W2" t="s">
         <v>108</v>
       </c>
-      <c r="W2" t="s">
+      <c r="X2" t="s">
         <v>109</v>
       </c>
-      <c r="X2" t="s">
+      <c r="Y2" t="s">
         <v>110</v>
       </c>
-      <c r="Y2" t="s">
+      <c r="Z2" t="s">
         <v>111</v>
       </c>
-      <c r="Z2" t="s">
+      <c r="AA2" t="s">
         <v>112</v>
       </c>
-      <c r="AA2" t="s">
+      <c r="AB2" t="s">
         <v>113</v>
       </c>
-      <c r="AB2" t="s">
+      <c r="AC2" t="s">
         <v>114</v>
       </c>
-      <c r="AC2" t="s">
+      <c r="AD2" t="s">
         <v>115</v>
       </c>
-      <c r="AD2" t="s">
+      <c r="AE2" t="s">
         <v>116</v>
       </c>
-      <c r="AE2" t="s">
+      <c r="AF2" t="s">
         <v>117</v>
       </c>
-      <c r="AF2" t="s">
+      <c r="AG2" t="s">
         <v>118</v>
       </c>
-      <c r="AG2" t="s">
+      <c r="AH2" t="s">
         <v>119</v>
       </c>
-      <c r="AH2" t="s">
+      <c r="AI2" t="s">
         <v>120</v>
       </c>
-      <c r="AI2" t="s">
+      <c r="AJ2" t="s">
         <v>121</v>
       </c>
-      <c r="AJ2" t="s">
+      <c r="AK2" t="s">
         <v>122</v>
       </c>
-      <c r="AK2" t="s">
+      <c r="AL2" t="s">
         <v>123</v>
       </c>
-      <c r="AL2" t="s">
+      <c r="AM2" t="s">
         <v>124</v>
       </c>
-      <c r="AM2" t="s">
+      <c r="AN2" t="s">
         <v>125</v>
       </c>
-      <c r="AN2" t="s">
+      <c r="AO2" t="s">
         <v>126</v>
       </c>
-      <c r="AO2" t="s">
+      <c r="AP2" t="s">
         <v>127</v>
       </c>
-      <c r="AP2" t="s">
+      <c r="AQ2" t="s">
         <v>128</v>
       </c>
-      <c r="AQ2" t="s">
+      <c r="AR2" t="s">
         <v>129</v>
       </c>
-      <c r="AR2" t="s">
+      <c r="AS2" t="s">
         <v>130</v>
       </c>
-      <c r="AS2" t="s">
+      <c r="AT2" t="s">
         <v>131</v>
       </c>
-      <c r="AT2" t="s">
+      <c r="AU2" t="s">
         <v>132</v>
       </c>
-      <c r="AU2" t="s">
+      <c r="AV2" t="s">
         <v>133</v>
       </c>
-      <c r="AV2" t="s">
+      <c r="AW2" t="s">
         <v>134</v>
-      </c>
-      <c r="AW2" t="s">
-        <v>135</v>
       </c>
     </row>
     <row r="3" spans="1:49">
@@ -1786,10 +1777,10 @@
         <v>12</v>
       </c>
       <c r="B3" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D3">
         <v>16062016</v>
@@ -1798,7 +1789,7 @@
         <v>1</v>
       </c>
       <c r="F3" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="G3">
         <v>2</v>
@@ -1953,28 +1944,28 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C2" t="s">
+        <v>136</v>
+      </c>
+      <c r="D2" t="s">
         <v>137</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>138</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F2" t="s">
         <v>139</v>
       </c>
-      <c r="F2" t="s">
+      <c r="G2" t="s">
         <v>140</v>
       </c>
-      <c r="G2" t="s">
+      <c r="H2" t="s">
         <v>141</v>
       </c>
-      <c r="H2" t="s">
+      <c r="I2" t="s">
         <v>142</v>
-      </c>
-      <c r="I2" t="s">
-        <v>143</v>
       </c>
     </row>
     <row r="3" spans="1:9">
@@ -1982,7 +1973,7 @@
         <v>12</v>
       </c>
       <c r="B3" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C3">
         <v>8</v>
@@ -2003,7 +1994,7 @@
         <v>1</v>
       </c>
       <c r="I3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="4" spans="1:9">
@@ -2011,7 +2002,7 @@
         <v>12</v>
       </c>
       <c r="B4" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="C4">
         <v>2</v>
@@ -2029,7 +2020,7 @@
         <v>1</v>
       </c>
       <c r="I4" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="5" spans="1:9">
@@ -2037,7 +2028,7 @@
         <v>12</v>
       </c>
       <c r="B5" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="C5">
         <v>2</v>

</xml_diff>

<commit_message>
Updated example csv files to add in collection occasion scores.
</commit_message>
<xml_diff>
--- a/data/_orig/pmhc-upload.xlsx
+++ b/data/_orig/pmhc-upload.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="198" uniqueCount="146">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="228" uniqueCount="167">
   <si>
     <t>Version</t>
   </si>
@@ -73,6 +73,15 @@
     <t>CL02</t>
   </si>
   <si>
+    <t>Y6D675D85QB6EAPE48TZYDWWS2WZP1G7</t>
+  </si>
+  <si>
+    <t>CL03</t>
+  </si>
+  <si>
+    <t>TJMQXZYD7EDZP2VRW3E3S51ME2JR12ZH</t>
+  </si>
+  <si>
     <t>episode_key</t>
   </si>
   <si>
@@ -157,6 +166,15 @@
     <t>tag3</t>
   </si>
   <si>
+    <t>E02</t>
+  </si>
+  <si>
+    <t>E03</t>
+  </si>
+  <si>
+    <t>E04</t>
+  </si>
+  <si>
     <t>service_contact_key</t>
   </si>
   <si>
@@ -265,6 +283,9 @@
     <t>k10p_item14</t>
   </si>
   <si>
+    <t>k10p_score</t>
+  </si>
+  <si>
     <t>k10p_tags</t>
   </si>
   <si>
@@ -274,6 +295,9 @@
     <t>CO02</t>
   </si>
   <si>
+    <t>CO03</t>
+  </si>
+  <si>
     <t>k5_item1</t>
   </si>
   <si>
@@ -289,12 +313,21 @@
     <t>k5_item5</t>
   </si>
   <si>
+    <t>k5_score</t>
+  </si>
+  <si>
     <t>k5_tags</t>
   </si>
   <si>
+    <t>CO04</t>
+  </si>
+  <si>
     <t>tag1 tag2</t>
   </si>
   <si>
+    <t>CO05</t>
+  </si>
+  <si>
     <t>sdq_version</t>
   </si>
   <si>
@@ -424,10 +457,40 @@
     <t>sdq_item42</t>
   </si>
   <si>
+    <t>sdq_emotional_symptoms</t>
+  </si>
+  <si>
+    <t>sdq_conduct_problem</t>
+  </si>
+  <si>
+    <t>sdq_hyperactivity</t>
+  </si>
+  <si>
+    <t>sdq_peer_problem</t>
+  </si>
+  <si>
+    <t>sdq_prosocial</t>
+  </si>
+  <si>
+    <t>sdq_total</t>
+  </si>
+  <si>
+    <t>sdq_impact</t>
+  </si>
+  <si>
     <t>sdq_tags</t>
   </si>
   <si>
+    <t>CO06</t>
+  </si>
+  <si>
     <t>PC101</t>
+  </si>
+  <si>
+    <t>CO07</t>
+  </si>
+  <si>
+    <t>PC201</t>
   </si>
   <si>
     <t>practitioner_category</t>
@@ -789,7 +852,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:K4"/>
+  <dimension ref="A1:K5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -881,13 +944,13 @@
         <v>16</v>
       </c>
       <c r="C4" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="D4">
-        <v>28021983</v>
+        <v>15062006</v>
       </c>
       <c r="E4">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F4">
         <v>2</v>
@@ -902,7 +965,39 @@
         <v>1201</v>
       </c>
       <c r="J4">
-        <v>3</v>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11">
+      <c r="A5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B5" t="s">
+        <v>18</v>
+      </c>
+      <c r="C5" t="s">
+        <v>19</v>
+      </c>
+      <c r="D5">
+        <v>21081996</v>
+      </c>
+      <c r="E5">
+        <v>1</v>
+      </c>
+      <c r="F5">
+        <v>1</v>
+      </c>
+      <c r="G5">
+        <v>1</v>
+      </c>
+      <c r="H5">
+        <v>1101</v>
+      </c>
+      <c r="I5">
+        <v>8911</v>
+      </c>
+      <c r="J5">
+        <v>4</v>
       </c>
     </row>
   </sheetData>
@@ -912,7 +1007,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:AB3"/>
+  <dimension ref="A1:AB6"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -931,85 +1026,85 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="C2" t="s">
         <v>2</v>
       </c>
       <c r="D2" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="E2" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="F2" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="G2" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="H2" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="I2" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="J2" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="K2" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="L2" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="M2" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="N2" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="O2" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="P2" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="Q2" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="R2" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="S2" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="T2" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="U2" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="V2" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="W2" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="X2" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="Y2" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="Z2" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="AA2" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="AB2" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
     </row>
     <row r="3" spans="1:28">
@@ -1017,7 +1112,7 @@
         <v>12</v>
       </c>
       <c r="B3" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="C3" t="s">
         <v>13</v>
@@ -1038,7 +1133,7 @@
         <v>2</v>
       </c>
       <c r="I3">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="J3">
         <v>1</v>
@@ -1047,7 +1142,7 @@
         <v>1101</v>
       </c>
       <c r="L3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="M3">
         <v>1</v>
@@ -1095,7 +1190,238 @@
         <v>1</v>
       </c>
       <c r="AB3" t="s">
-        <v>44</v>
+        <v>47</v>
+      </c>
+    </row>
+    <row r="4" spans="1:28">
+      <c r="A4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B4" t="s">
+        <v>48</v>
+      </c>
+      <c r="C4" t="s">
+        <v>13</v>
+      </c>
+      <c r="D4">
+        <v>16082016</v>
+      </c>
+      <c r="E4">
+        <v>1</v>
+      </c>
+      <c r="F4">
+        <v>2</v>
+      </c>
+      <c r="G4">
+        <v>14072016</v>
+      </c>
+      <c r="H4">
+        <v>2</v>
+      </c>
+      <c r="I4">
+        <v>3</v>
+      </c>
+      <c r="J4">
+        <v>1</v>
+      </c>
+      <c r="K4">
+        <v>1101</v>
+      </c>
+      <c r="L4">
+        <v>2</v>
+      </c>
+      <c r="M4">
+        <v>1</v>
+      </c>
+      <c r="N4">
+        <v>2</v>
+      </c>
+      <c r="O4">
+        <v>2</v>
+      </c>
+      <c r="P4">
+        <v>2</v>
+      </c>
+      <c r="Q4">
+        <v>1</v>
+      </c>
+      <c r="R4">
+        <v>2</v>
+      </c>
+      <c r="S4">
+        <v>107</v>
+      </c>
+      <c r="T4">
+        <v>903</v>
+      </c>
+      <c r="U4">
+        <v>2</v>
+      </c>
+      <c r="V4">
+        <v>2</v>
+      </c>
+      <c r="W4">
+        <v>2</v>
+      </c>
+      <c r="X4">
+        <v>2</v>
+      </c>
+      <c r="Y4">
+        <v>2</v>
+      </c>
+      <c r="Z4">
+        <v>2</v>
+      </c>
+      <c r="AA4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:28">
+      <c r="A5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B5" t="s">
+        <v>49</v>
+      </c>
+      <c r="C5" t="s">
+        <v>16</v>
+      </c>
+      <c r="E5">
+        <v>1</v>
+      </c>
+      <c r="G5">
+        <v>10062016</v>
+      </c>
+      <c r="H5">
+        <v>5</v>
+      </c>
+      <c r="I5">
+        <v>2</v>
+      </c>
+      <c r="J5">
+        <v>3</v>
+      </c>
+      <c r="K5">
+        <v>1102</v>
+      </c>
+      <c r="L5">
+        <v>3</v>
+      </c>
+      <c r="M5">
+        <v>3</v>
+      </c>
+      <c r="N5">
+        <v>6</v>
+      </c>
+      <c r="O5">
+        <v>1</v>
+      </c>
+      <c r="P5">
+        <v>1</v>
+      </c>
+      <c r="Q5">
+        <v>1</v>
+      </c>
+      <c r="R5">
+        <v>2</v>
+      </c>
+      <c r="S5">
+        <v>502</v>
+      </c>
+      <c r="U5">
+        <v>2</v>
+      </c>
+      <c r="V5">
+        <v>2</v>
+      </c>
+      <c r="W5">
+        <v>2</v>
+      </c>
+      <c r="X5">
+        <v>2</v>
+      </c>
+      <c r="Y5">
+        <v>2</v>
+      </c>
+      <c r="Z5">
+        <v>2</v>
+      </c>
+      <c r="AA5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:28">
+      <c r="A6" t="s">
+        <v>12</v>
+      </c>
+      <c r="B6" t="s">
+        <v>50</v>
+      </c>
+      <c r="C6" t="s">
+        <v>18</v>
+      </c>
+      <c r="E6">
+        <v>1</v>
+      </c>
+      <c r="G6">
+        <v>23042016</v>
+      </c>
+      <c r="H6">
+        <v>6</v>
+      </c>
+      <c r="I6">
+        <v>2</v>
+      </c>
+      <c r="J6">
+        <v>3</v>
+      </c>
+      <c r="K6">
+        <v>1102</v>
+      </c>
+      <c r="L6">
+        <v>2</v>
+      </c>
+      <c r="M6">
+        <v>3</v>
+      </c>
+      <c r="N6">
+        <v>2</v>
+      </c>
+      <c r="O6">
+        <v>1</v>
+      </c>
+      <c r="P6">
+        <v>2</v>
+      </c>
+      <c r="Q6">
+        <v>5</v>
+      </c>
+      <c r="R6">
+        <v>2</v>
+      </c>
+      <c r="S6">
+        <v>901</v>
+      </c>
+      <c r="U6">
+        <v>2</v>
+      </c>
+      <c r="V6">
+        <v>2</v>
+      </c>
+      <c r="W6">
+        <v>2</v>
+      </c>
+      <c r="X6">
+        <v>1</v>
+      </c>
+      <c r="Y6">
+        <v>2</v>
+      </c>
+      <c r="Z6">
+        <v>10</v>
+      </c>
+      <c r="AA6">
+        <v>4</v>
       </c>
     </row>
   </sheetData>
@@ -1124,52 +1450,52 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>45</v>
+        <v>51</v>
       </c>
       <c r="C2" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="D2" t="s">
-        <v>46</v>
+        <v>52</v>
       </c>
       <c r="E2" t="s">
-        <v>47</v>
+        <v>53</v>
       </c>
       <c r="F2" t="s">
-        <v>48</v>
+        <v>54</v>
       </c>
       <c r="G2" t="s">
-        <v>49</v>
+        <v>55</v>
       </c>
       <c r="H2" t="s">
-        <v>50</v>
+        <v>56</v>
       </c>
       <c r="I2" t="s">
-        <v>51</v>
+        <v>57</v>
       </c>
       <c r="J2" t="s">
-        <v>52</v>
+        <v>58</v>
       </c>
       <c r="K2" t="s">
-        <v>53</v>
+        <v>59</v>
       </c>
       <c r="L2" t="s">
-        <v>54</v>
+        <v>60</v>
       </c>
       <c r="M2" t="s">
-        <v>55</v>
+        <v>61</v>
       </c>
       <c r="N2" t="s">
-        <v>56</v>
+        <v>62</v>
       </c>
       <c r="O2" t="s">
-        <v>57</v>
+        <v>63</v>
       </c>
       <c r="P2" t="s">
-        <v>58</v>
+        <v>64</v>
       </c>
       <c r="Q2" t="s">
-        <v>59</v>
+        <v>65</v>
       </c>
     </row>
     <row r="3" spans="1:17">
@@ -1177,16 +1503,16 @@
         <v>12</v>
       </c>
       <c r="B3" t="s">
-        <v>60</v>
+        <v>66</v>
       </c>
       <c r="C3" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="D3" t="s">
-        <v>61</v>
+        <v>67</v>
       </c>
       <c r="E3">
-        <v>18062016</v>
+        <v>13022016</v>
       </c>
       <c r="F3">
         <v>1</v>
@@ -1227,16 +1553,16 @@
         <v>12</v>
       </c>
       <c r="B4" t="s">
-        <v>62</v>
+        <v>68</v>
       </c>
       <c r="C4" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="D4" t="s">
-        <v>61</v>
+        <v>67</v>
       </c>
       <c r="E4">
-        <v>18062016</v>
+        <v>18032016</v>
       </c>
       <c r="F4">
         <v>1</v>
@@ -1272,7 +1598,7 @@
         <v>3</v>
       </c>
       <c r="Q4" t="s">
-        <v>63</v>
+        <v>69</v>
       </c>
     </row>
   </sheetData>
@@ -1282,13 +1608,13 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:T4"/>
+  <dimension ref="A1:U5"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:20">
+    <row r="1" spans="1:21">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1296,80 +1622,83 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:20">
+    <row r="2" spans="1:21">
       <c r="A2" t="s">
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>64</v>
+        <v>70</v>
       </c>
       <c r="C2" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="D2" t="s">
-        <v>65</v>
+        <v>71</v>
       </c>
       <c r="E2" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="F2" t="s">
-        <v>67</v>
+        <v>73</v>
       </c>
       <c r="G2" t="s">
-        <v>68</v>
+        <v>74</v>
       </c>
       <c r="H2" t="s">
-        <v>69</v>
+        <v>75</v>
       </c>
       <c r="I2" t="s">
-        <v>70</v>
+        <v>76</v>
       </c>
       <c r="J2" t="s">
-        <v>71</v>
+        <v>77</v>
       </c>
       <c r="K2" t="s">
-        <v>72</v>
+        <v>78</v>
       </c>
       <c r="L2" t="s">
-        <v>73</v>
+        <v>79</v>
       </c>
       <c r="M2" t="s">
-        <v>74</v>
+        <v>80</v>
       </c>
       <c r="N2" t="s">
-        <v>75</v>
+        <v>81</v>
       </c>
       <c r="O2" t="s">
-        <v>76</v>
+        <v>82</v>
       </c>
       <c r="P2" t="s">
-        <v>77</v>
+        <v>83</v>
       </c>
       <c r="Q2" t="s">
-        <v>78</v>
+        <v>84</v>
       </c>
       <c r="R2" t="s">
-        <v>79</v>
+        <v>85</v>
       </c>
       <c r="S2" t="s">
-        <v>80</v>
+        <v>86</v>
       </c>
       <c r="T2" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="3" spans="1:20">
+        <v>87</v>
+      </c>
+      <c r="U2" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="3" spans="1:21">
       <c r="A3" t="s">
         <v>12</v>
       </c>
       <c r="B3" t="s">
-        <v>82</v>
+        <v>89</v>
       </c>
       <c r="C3" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="D3">
-        <v>18062016</v>
+        <v>12022016</v>
       </c>
       <c r="E3">
         <v>1</v>
@@ -1416,19 +1745,22 @@
       <c r="S3">
         <v>4</v>
       </c>
-    </row>
-    <row r="4" spans="1:20">
+      <c r="T3">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="4" spans="1:21">
       <c r="A4" t="s">
         <v>12</v>
       </c>
       <c r="B4" t="s">
-        <v>83</v>
+        <v>90</v>
       </c>
       <c r="C4" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="D4">
-        <v>18062016</v>
+        <v>25042016</v>
       </c>
       <c r="E4">
         <v>2</v>
@@ -1475,8 +1807,46 @@
       <c r="S4">
         <v>3</v>
       </c>
-      <c r="T4" t="s">
-        <v>63</v>
+      <c r="T4">
+        <v>99</v>
+      </c>
+      <c r="U4" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="5" spans="1:21">
+      <c r="A5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B5" t="s">
+        <v>91</v>
+      </c>
+      <c r="C5" t="s">
+        <v>46</v>
+      </c>
+      <c r="D5">
+        <v>18062016</v>
+      </c>
+      <c r="E5">
+        <v>3</v>
+      </c>
+      <c r="P5">
+        <v>1</v>
+      </c>
+      <c r="Q5">
+        <v>3</v>
+      </c>
+      <c r="R5">
+        <v>1</v>
+      </c>
+      <c r="S5">
+        <v>2</v>
+      </c>
+      <c r="T5">
+        <v>25</v>
+      </c>
+      <c r="U5" t="s">
+        <v>69</v>
       </c>
     </row>
   </sheetData>
@@ -1486,13 +1856,13 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:K4"/>
+  <dimension ref="A1:L4"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:11">
+    <row r="1" spans="1:12">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1500,56 +1870,59 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:11">
+    <row r="2" spans="1:12">
       <c r="A2" t="s">
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>64</v>
+        <v>70</v>
       </c>
       <c r="C2" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="D2" t="s">
-        <v>65</v>
+        <v>71</v>
       </c>
       <c r="E2" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="F2" t="s">
-        <v>84</v>
+        <v>92</v>
       </c>
       <c r="G2" t="s">
-        <v>85</v>
+        <v>93</v>
       </c>
       <c r="H2" t="s">
-        <v>86</v>
+        <v>94</v>
       </c>
       <c r="I2" t="s">
-        <v>87</v>
+        <v>95</v>
       </c>
       <c r="J2" t="s">
-        <v>88</v>
+        <v>96</v>
       </c>
       <c r="K2" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11">
+        <v>97</v>
+      </c>
+      <c r="L2" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12">
       <c r="A3" t="s">
         <v>12</v>
       </c>
       <c r="B3" t="s">
-        <v>82</v>
+        <v>99</v>
       </c>
       <c r="C3" t="s">
-        <v>43</v>
+        <v>50</v>
       </c>
       <c r="D3">
-        <v>18062016</v>
+        <v>24042016</v>
       </c>
       <c r="E3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F3">
         <v>1</v>
@@ -1566,40 +1939,34 @@
       <c r="J3">
         <v>5</v>
       </c>
-      <c r="K3" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11">
+      <c r="K3">
+        <v>99</v>
+      </c>
+      <c r="L3" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12">
       <c r="A4" t="s">
         <v>12</v>
       </c>
       <c r="B4" t="s">
-        <v>83</v>
+        <v>101</v>
       </c>
       <c r="C4" t="s">
-        <v>43</v>
+        <v>50</v>
       </c>
       <c r="D4">
-        <v>18062016</v>
+        <v>19062016</v>
       </c>
       <c r="E4">
         <v>2</v>
       </c>
-      <c r="F4">
-        <v>3</v>
-      </c>
-      <c r="G4">
-        <v>1</v>
-      </c>
-      <c r="H4">
-        <v>1</v>
-      </c>
-      <c r="I4">
-        <v>1</v>
-      </c>
-      <c r="J4">
-        <v>4</v>
+      <c r="K4">
+        <v>20</v>
+      </c>
+      <c r="L4" t="s">
+        <v>100</v>
       </c>
     </row>
   </sheetData>
@@ -1609,13 +1976,13 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:AW3"/>
+  <dimension ref="A1:BD4"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:49">
+    <row r="1" spans="1:56">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1623,164 +1990,185 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:49">
+    <row r="2" spans="1:56">
       <c r="A2" t="s">
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>64</v>
+        <v>70</v>
       </c>
       <c r="C2" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="D2" t="s">
-        <v>65</v>
+        <v>71</v>
       </c>
       <c r="E2" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="F2" t="s">
-        <v>91</v>
+        <v>102</v>
       </c>
       <c r="G2" t="s">
-        <v>92</v>
+        <v>103</v>
       </c>
       <c r="H2" t="s">
-        <v>93</v>
+        <v>104</v>
       </c>
       <c r="I2" t="s">
-        <v>94</v>
+        <v>105</v>
       </c>
       <c r="J2" t="s">
-        <v>95</v>
+        <v>106</v>
       </c>
       <c r="K2" t="s">
-        <v>96</v>
+        <v>107</v>
       </c>
       <c r="L2" t="s">
-        <v>97</v>
+        <v>108</v>
       </c>
       <c r="M2" t="s">
-        <v>98</v>
+        <v>109</v>
       </c>
       <c r="N2" t="s">
-        <v>99</v>
+        <v>110</v>
       </c>
       <c r="O2" t="s">
-        <v>100</v>
+        <v>111</v>
       </c>
       <c r="P2" t="s">
-        <v>101</v>
+        <v>112</v>
       </c>
       <c r="Q2" t="s">
-        <v>102</v>
+        <v>113</v>
       </c>
       <c r="R2" t="s">
-        <v>103</v>
+        <v>114</v>
       </c>
       <c r="S2" t="s">
-        <v>104</v>
+        <v>115</v>
       </c>
       <c r="T2" t="s">
-        <v>105</v>
+        <v>116</v>
       </c>
       <c r="U2" t="s">
-        <v>106</v>
+        <v>117</v>
       </c>
       <c r="V2" t="s">
-        <v>107</v>
+        <v>118</v>
       </c>
       <c r="W2" t="s">
-        <v>108</v>
+        <v>119</v>
       </c>
       <c r="X2" t="s">
-        <v>109</v>
+        <v>120</v>
       </c>
       <c r="Y2" t="s">
-        <v>110</v>
+        <v>121</v>
       </c>
       <c r="Z2" t="s">
-        <v>111</v>
+        <v>122</v>
       </c>
       <c r="AA2" t="s">
-        <v>112</v>
+        <v>123</v>
       </c>
       <c r="AB2" t="s">
-        <v>113</v>
+        <v>124</v>
       </c>
       <c r="AC2" t="s">
-        <v>114</v>
+        <v>125</v>
       </c>
       <c r="AD2" t="s">
-        <v>115</v>
+        <v>126</v>
       </c>
       <c r="AE2" t="s">
-        <v>116</v>
+        <v>127</v>
       </c>
       <c r="AF2" t="s">
-        <v>117</v>
+        <v>128</v>
       </c>
       <c r="AG2" t="s">
-        <v>118</v>
+        <v>129</v>
       </c>
       <c r="AH2" t="s">
-        <v>119</v>
+        <v>130</v>
       </c>
       <c r="AI2" t="s">
-        <v>120</v>
+        <v>131</v>
       </c>
       <c r="AJ2" t="s">
-        <v>121</v>
+        <v>132</v>
       </c>
       <c r="AK2" t="s">
-        <v>122</v>
+        <v>133</v>
       </c>
       <c r="AL2" t="s">
-        <v>123</v>
+        <v>134</v>
       </c>
       <c r="AM2" t="s">
-        <v>124</v>
+        <v>135</v>
       </c>
       <c r="AN2" t="s">
-        <v>125</v>
+        <v>136</v>
       </c>
       <c r="AO2" t="s">
-        <v>126</v>
+        <v>137</v>
       </c>
       <c r="AP2" t="s">
-        <v>127</v>
+        <v>138</v>
       </c>
       <c r="AQ2" t="s">
-        <v>128</v>
+        <v>139</v>
       </c>
       <c r="AR2" t="s">
-        <v>129</v>
+        <v>140</v>
       </c>
       <c r="AS2" t="s">
-        <v>130</v>
+        <v>141</v>
       </c>
       <c r="AT2" t="s">
-        <v>131</v>
+        <v>142</v>
       </c>
       <c r="AU2" t="s">
-        <v>132</v>
+        <v>143</v>
       </c>
       <c r="AV2" t="s">
-        <v>133</v>
+        <v>144</v>
       </c>
       <c r="AW2" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="3" spans="1:49">
+        <v>145</v>
+      </c>
+      <c r="AX2" t="s">
+        <v>146</v>
+      </c>
+      <c r="AY2" t="s">
+        <v>147</v>
+      </c>
+      <c r="AZ2" t="s">
+        <v>148</v>
+      </c>
+      <c r="BA2" t="s">
+        <v>149</v>
+      </c>
+      <c r="BB2" t="s">
+        <v>150</v>
+      </c>
+      <c r="BC2" t="s">
+        <v>151</v>
+      </c>
+      <c r="BD2" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="3" spans="1:56">
       <c r="A3" t="s">
         <v>12</v>
       </c>
       <c r="B3" t="s">
-        <v>82</v>
+        <v>153</v>
       </c>
       <c r="C3" t="s">
-        <v>43</v>
+        <v>49</v>
       </c>
       <c r="D3">
         <v>16062016</v>
@@ -1789,7 +2177,7 @@
         <v>1</v>
       </c>
       <c r="F3" t="s">
-        <v>135</v>
+        <v>154</v>
       </c>
       <c r="G3">
         <v>2</v>
@@ -1916,6 +2304,68 @@
       </c>
       <c r="AV3">
         <v>0</v>
+      </c>
+      <c r="AW3">
+        <v>99</v>
+      </c>
+      <c r="AX3">
+        <v>99</v>
+      </c>
+      <c r="AY3">
+        <v>99</v>
+      </c>
+      <c r="AZ3">
+        <v>99</v>
+      </c>
+      <c r="BA3">
+        <v>99</v>
+      </c>
+      <c r="BB3">
+        <v>99</v>
+      </c>
+      <c r="BC3">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="4" spans="1:56">
+      <c r="A4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B4" t="s">
+        <v>155</v>
+      </c>
+      <c r="C4" t="s">
+        <v>49</v>
+      </c>
+      <c r="D4">
+        <v>11072016</v>
+      </c>
+      <c r="E4">
+        <v>2</v>
+      </c>
+      <c r="F4" t="s">
+        <v>156</v>
+      </c>
+      <c r="AW4">
+        <v>2</v>
+      </c>
+      <c r="AX4">
+        <v>3</v>
+      </c>
+      <c r="AY4">
+        <v>3</v>
+      </c>
+      <c r="AZ4">
+        <v>2</v>
+      </c>
+      <c r="BA4">
+        <v>3</v>
+      </c>
+      <c r="BB4">
+        <v>13</v>
+      </c>
+      <c r="BC4">
+        <v>5</v>
       </c>
     </row>
   </sheetData>
@@ -1944,28 +2394,28 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>46</v>
+        <v>52</v>
       </c>
       <c r="C2" t="s">
-        <v>136</v>
+        <v>157</v>
       </c>
       <c r="D2" t="s">
-        <v>137</v>
+        <v>158</v>
       </c>
       <c r="E2" t="s">
-        <v>138</v>
+        <v>159</v>
       </c>
       <c r="F2" t="s">
-        <v>139</v>
+        <v>160</v>
       </c>
       <c r="G2" t="s">
-        <v>140</v>
+        <v>161</v>
       </c>
       <c r="H2" t="s">
-        <v>141</v>
+        <v>162</v>
       </c>
       <c r="I2" t="s">
-        <v>142</v>
+        <v>163</v>
       </c>
     </row>
     <row r="3" spans="1:9">
@@ -1973,7 +2423,7 @@
         <v>12</v>
       </c>
       <c r="B3" t="s">
-        <v>61</v>
+        <v>67</v>
       </c>
       <c r="C3">
         <v>8</v>
@@ -1994,7 +2444,7 @@
         <v>1</v>
       </c>
       <c r="I3" t="s">
-        <v>63</v>
+        <v>69</v>
       </c>
     </row>
     <row r="4" spans="1:9">
@@ -2002,7 +2452,7 @@
         <v>12</v>
       </c>
       <c r="B4" t="s">
-        <v>143</v>
+        <v>164</v>
       </c>
       <c r="C4">
         <v>2</v>
@@ -2020,7 +2470,7 @@
         <v>1</v>
       </c>
       <c r="I4" t="s">
-        <v>144</v>
+        <v>165</v>
       </c>
     </row>
     <row r="5" spans="1:9">
@@ -2028,7 +2478,7 @@
         <v>12</v>
       </c>
       <c r="B5" t="s">
-        <v>145</v>
+        <v>166</v>
       </c>
       <c r="C5">
         <v>2</v>

</xml_diff>

<commit_message>
Updated excel example file.
</commit_message>
<xml_diff>
--- a/data/_orig/pmhc-upload.xlsx
+++ b/data/_orig/pmhc-upload.xlsx
@@ -927,7 +927,7 @@
         <v>1102</v>
       </c>
       <c r="I3">
-        <v>1202</v>
+        <v>1201</v>
       </c>
       <c r="J3">
         <v>3</v>
@@ -1328,6 +1328,9 @@
       <c r="S5">
         <v>502</v>
       </c>
+      <c r="T5">
+        <v>999</v>
+      </c>
       <c r="U5">
         <v>2</v>
       </c>
@@ -1401,6 +1404,9 @@
       </c>
       <c r="S6">
         <v>901</v>
+      </c>
+      <c r="T6">
+        <v>999</v>
       </c>
       <c r="U6">
         <v>2</v>
@@ -1830,6 +1836,36 @@
       <c r="E5">
         <v>3</v>
       </c>
+      <c r="F5">
+        <v>9</v>
+      </c>
+      <c r="G5">
+        <v>9</v>
+      </c>
+      <c r="H5">
+        <v>9</v>
+      </c>
+      <c r="I5">
+        <v>9</v>
+      </c>
+      <c r="J5">
+        <v>9</v>
+      </c>
+      <c r="K5">
+        <v>9</v>
+      </c>
+      <c r="L5">
+        <v>9</v>
+      </c>
+      <c r="M5">
+        <v>9</v>
+      </c>
+      <c r="N5">
+        <v>9</v>
+      </c>
+      <c r="O5">
+        <v>9</v>
+      </c>
       <c r="P5">
         <v>1</v>
       </c>
@@ -1962,6 +1998,21 @@
       <c r="E4">
         <v>2</v>
       </c>
+      <c r="F4">
+        <v>9</v>
+      </c>
+      <c r="G4">
+        <v>9</v>
+      </c>
+      <c r="H4">
+        <v>9</v>
+      </c>
+      <c r="I4">
+        <v>9</v>
+      </c>
+      <c r="J4">
+        <v>9</v>
+      </c>
       <c r="K4">
         <v>20</v>
       </c>
@@ -2346,6 +2397,132 @@
       <c r="F4" t="s">
         <v>156</v>
       </c>
+      <c r="G4">
+        <v>9</v>
+      </c>
+      <c r="H4">
+        <v>9</v>
+      </c>
+      <c r="I4">
+        <v>9</v>
+      </c>
+      <c r="J4">
+        <v>9</v>
+      </c>
+      <c r="K4">
+        <v>9</v>
+      </c>
+      <c r="L4">
+        <v>9</v>
+      </c>
+      <c r="M4">
+        <v>9</v>
+      </c>
+      <c r="N4">
+        <v>9</v>
+      </c>
+      <c r="O4">
+        <v>9</v>
+      </c>
+      <c r="P4">
+        <v>9</v>
+      </c>
+      <c r="Q4">
+        <v>9</v>
+      </c>
+      <c r="R4">
+        <v>9</v>
+      </c>
+      <c r="S4">
+        <v>9</v>
+      </c>
+      <c r="T4">
+        <v>9</v>
+      </c>
+      <c r="U4">
+        <v>9</v>
+      </c>
+      <c r="V4">
+        <v>9</v>
+      </c>
+      <c r="W4">
+        <v>9</v>
+      </c>
+      <c r="X4">
+        <v>9</v>
+      </c>
+      <c r="Y4">
+        <v>9</v>
+      </c>
+      <c r="Z4">
+        <v>9</v>
+      </c>
+      <c r="AA4">
+        <v>9</v>
+      </c>
+      <c r="AB4">
+        <v>9</v>
+      </c>
+      <c r="AC4">
+        <v>9</v>
+      </c>
+      <c r="AD4">
+        <v>9</v>
+      </c>
+      <c r="AE4">
+        <v>9</v>
+      </c>
+      <c r="AF4">
+        <v>9</v>
+      </c>
+      <c r="AG4">
+        <v>9</v>
+      </c>
+      <c r="AH4">
+        <v>9</v>
+      </c>
+      <c r="AI4">
+        <v>9</v>
+      </c>
+      <c r="AJ4">
+        <v>9</v>
+      </c>
+      <c r="AK4">
+        <v>9</v>
+      </c>
+      <c r="AL4">
+        <v>9</v>
+      </c>
+      <c r="AM4">
+        <v>9</v>
+      </c>
+      <c r="AN4">
+        <v>9</v>
+      </c>
+      <c r="AO4">
+        <v>9</v>
+      </c>
+      <c r="AP4">
+        <v>9</v>
+      </c>
+      <c r="AQ4">
+        <v>9</v>
+      </c>
+      <c r="AR4">
+        <v>9</v>
+      </c>
+      <c r="AS4">
+        <v>9</v>
+      </c>
+      <c r="AT4">
+        <v>9</v>
+      </c>
+      <c r="AU4">
+        <v>9</v>
+      </c>
+      <c r="AV4">
+        <v>9</v>
+      </c>
       <c r="AW4">
         <v>2</v>
       </c>

</xml_diff>

<commit_message>
Updating example upload files with ones that successfully validate.
</commit_message>
<xml_diff>
--- a/data/_orig/pmhc-upload.xlsx
+++ b/data/_orig/pmhc-upload.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
-  <workbookPr defaultThemeVersion="124226"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="28125"/>
+  <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="32120" windowHeight="16060" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="Clients" sheetId="1" r:id="rId1"/>
@@ -15,12 +15,17 @@
     <sheet name="SDQ" sheetId="6" r:id="rId6"/>
     <sheet name="Practitioners" sheetId="7" r:id="rId7"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="124519" concurrentCalc="0"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="228" uniqueCount="167">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="232" uniqueCount="167">
   <si>
     <t>Version</t>
   </si>
@@ -526,11 +531,34 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -553,13 +581,22 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="5">
+    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -851,12 +888,12 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView topLeftCell="A3" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <sheetData>
     <row r="1" spans="1:11">
       <c r="A1" t="s">
@@ -1002,16 +1039,21 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AB6"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <sheetData>
     <row r="1" spans="1:28">
       <c r="A1" t="s">
@@ -1432,16 +1474,23 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q4"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E13" sqref="E13"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <sheetData>
     <row r="1" spans="1:17">
       <c r="A1" t="s">
@@ -1609,16 +1658,34 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:U5"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:U6"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView topLeftCell="F2" workbookViewId="0">
+      <selection activeCell="L18" sqref="L18"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="1" max="1" width="15" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="14" width="10.1640625" bestFit="1" customWidth="1"/>
+    <col min="15" max="19" width="11.1640625" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="9.83203125" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="9" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:21">
       <c r="A1" t="s">
@@ -1831,10 +1898,10 @@
         <v>46</v>
       </c>
       <c r="D5">
-        <v>18062016</v>
+        <v>20052016</v>
       </c>
       <c r="E5">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F5">
         <v>9</v>
@@ -1867,13 +1934,13 @@
         <v>9</v>
       </c>
       <c r="P5">
-        <v>1</v>
+        <v>99</v>
       </c>
       <c r="Q5">
-        <v>3</v>
+        <v>99</v>
       </c>
       <c r="R5">
-        <v>1</v>
+        <v>99</v>
       </c>
       <c r="S5">
         <v>2</v>
@@ -1885,18 +1952,89 @@
         <v>69</v>
       </c>
     </row>
+    <row r="6" spans="1:21">
+      <c r="A6" t="s">
+        <v>12</v>
+      </c>
+      <c r="B6" t="s">
+        <v>99</v>
+      </c>
+      <c r="C6" t="s">
+        <v>46</v>
+      </c>
+      <c r="D6">
+        <v>18062016</v>
+      </c>
+      <c r="E6">
+        <v>3</v>
+      </c>
+      <c r="F6">
+        <v>1</v>
+      </c>
+      <c r="G6">
+        <v>1</v>
+      </c>
+      <c r="H6">
+        <v>1</v>
+      </c>
+      <c r="I6">
+        <v>1</v>
+      </c>
+      <c r="J6">
+        <v>1</v>
+      </c>
+      <c r="K6">
+        <v>1</v>
+      </c>
+      <c r="L6">
+        <v>1</v>
+      </c>
+      <c r="M6">
+        <v>1</v>
+      </c>
+      <c r="N6">
+        <v>1</v>
+      </c>
+      <c r="O6">
+        <v>1</v>
+      </c>
+      <c r="P6" s="1">
+        <v>1</v>
+      </c>
+      <c r="Q6" s="1">
+        <v>3</v>
+      </c>
+      <c r="R6" s="1">
+        <v>1</v>
+      </c>
+      <c r="S6">
+        <v>9</v>
+      </c>
+      <c r="T6">
+        <v>99</v>
+      </c>
+      <c r="U6" t="s">
+        <v>69</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L4"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <sheetData>
     <row r="1" spans="1:12">
       <c r="A1" t="s">
@@ -2022,16 +2160,41 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:BD4"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView topLeftCell="AD1" workbookViewId="0">
+      <selection activeCell="H14" sqref="H14"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="1" max="1" width="15" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="15" width="9.1640625" bestFit="1" customWidth="1"/>
+    <col min="16" max="48" width="10.1640625" bestFit="1" customWidth="1"/>
+    <col min="49" max="49" width="21.1640625" bestFit="1" customWidth="1"/>
+    <col min="50" max="50" width="18.1640625" bestFit="1" customWidth="1"/>
+    <col min="51" max="51" width="14.5" bestFit="1" customWidth="1"/>
+    <col min="52" max="52" width="15.5" bestFit="1" customWidth="1"/>
+    <col min="53" max="53" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="54" max="54" width="8.33203125" bestFit="1" customWidth="1"/>
+    <col min="55" max="55" width="10" bestFit="1" customWidth="1"/>
+    <col min="56" max="56" width="7.83203125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:56">
       <c r="A1" t="s">
@@ -2330,10 +2493,10 @@
         <v>2</v>
       </c>
       <c r="AN3">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="AO3">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="AP3">
         <v>0</v>
@@ -2345,16 +2508,16 @@
         <v>2</v>
       </c>
       <c r="AS3">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="AT3">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="AU3">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="AV3">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="AW3">
         <v>99</v>
@@ -2547,16 +2710,28 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I5"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H3" sqref="H3"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="1" max="1" width="15" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.6640625" customWidth="1"/>
+    <col min="6" max="7" width="17.5" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:9">
       <c r="A1" t="s">
@@ -2606,7 +2781,7 @@
         <v>8</v>
       </c>
       <c r="D3">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E3">
         <v>1975</v>
@@ -2634,6 +2809,9 @@
       <c r="C4">
         <v>2</v>
       </c>
+      <c r="D4">
+        <v>1</v>
+      </c>
       <c r="E4">
         <v>1977</v>
       </c>
@@ -2672,8 +2850,16 @@
       <c r="G5">
         <v>4</v>
       </c>
+      <c r="H5">
+        <v>0</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Updated example upload files to correct practitioners validation.
</commit_message>
<xml_diff>
--- a/data/_orig/pmhc-upload.xlsx
+++ b/data/_orig/pmhc-upload.xlsx
@@ -2723,7 +2723,7 @@
   <dimension ref="A1:I5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H3" sqref="H3"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -2781,7 +2781,7 @@
         <v>8</v>
       </c>
       <c r="D3">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E3">
         <v>1975</v>

</xml_diff>

<commit_message>
Added organistions into upload spec.
</commit_message>
<xml_diff>
--- a/data/_orig/pmhc-upload.xlsx
+++ b/data/_orig/pmhc-upload.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="28125"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="32120" windowHeight="16060" activeTab="6"/>
+    <workbookView xWindow="540" yWindow="2160" windowWidth="32120" windowHeight="16060" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="Clients" sheetId="1" r:id="rId1"/>
@@ -14,6 +14,7 @@
     <sheet name="K5" sheetId="5" r:id="rId5"/>
     <sheet name="SDQ" sheetId="6" r:id="rId6"/>
     <sheet name="Practitioners" sheetId="7" r:id="rId7"/>
+    <sheet name="Organisations" sheetId="8" r:id="rId8"/>
   </sheets>
   <calcPr calcId="124519" concurrentCalc="0"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="232" uniqueCount="167">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="245" uniqueCount="177">
   <si>
     <t>Version</t>
   </si>
@@ -526,6 +527,36 @@
   </si>
   <si>
     <t>P03</t>
+  </si>
+  <si>
+    <t>organisation_key</t>
+  </si>
+  <si>
+    <t>organisation_name</t>
+  </si>
+  <si>
+    <t>organisation_legal_name</t>
+  </si>
+  <si>
+    <t>organisation_abn</t>
+  </si>
+  <si>
+    <t>organisation_type</t>
+  </si>
+  <si>
+    <t>organisation_state</t>
+  </si>
+  <si>
+    <t>organisation_status</t>
+  </si>
+  <si>
+    <t>organisation_tags</t>
+  </si>
+  <si>
+    <t>NFP01</t>
+  </si>
+  <si>
+    <t>Test Provider Organisation NFP1</t>
   </si>
 </sst>
 </file>
@@ -894,6 +925,9 @@
     <sheetView topLeftCell="A3" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="1" max="1" width="15.1640625" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:11">
       <c r="A1" t="s">
@@ -2722,7 +2756,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
@@ -2862,4 +2896,91 @@
     </ext>
   </extLst>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:I3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F4" sqref="F4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="1" max="1" width="19.5" customWidth="1"/>
+    <col min="2" max="2" width="17.83203125" customWidth="1"/>
+    <col min="3" max="3" width="25.6640625" customWidth="1"/>
+    <col min="4" max="4" width="21.6640625" customWidth="1"/>
+    <col min="5" max="5" width="20.5" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9">
+      <c r="A2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>167</v>
+      </c>
+      <c r="C2" t="s">
+        <v>168</v>
+      </c>
+      <c r="D2" t="s">
+        <v>169</v>
+      </c>
+      <c r="E2" t="s">
+        <v>170</v>
+      </c>
+      <c r="F2" t="s">
+        <v>171</v>
+      </c>
+      <c r="G2" t="s">
+        <v>172</v>
+      </c>
+      <c r="H2" t="s">
+        <v>173</v>
+      </c>
+      <c r="I2" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9">
+      <c r="A3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B3" t="s">
+        <v>175</v>
+      </c>
+      <c r="C3" t="s">
+        <v>176</v>
+      </c>
+      <c r="E3">
+        <v>42072953425</v>
+      </c>
+      <c r="F3">
+        <v>7</v>
+      </c>
+      <c r="G3">
+        <v>1</v>
+      </c>
+      <c r="H3">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Cleanup sample PMHC 2.0 spec data
* Remove organisation omsss email
* Correct SDQ scores
</commit_message>
<xml_diff>
--- a/data/_orig/pmhc-upload.xlsx
+++ b/data/_orig/pmhc-upload.xlsx
@@ -5,12 +5,12 @@
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jenni/Work/git/PMHC/spec/data/_orig/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/russellj/stratdat/pmhc/spec/data/_orig/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5CAA1B3C-1363-664E-849A-8C351EDAE5D9}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF7E0106-773B-EB4D-B0A3-367B96F308D7}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38860" yWindow="3780" windowWidth="32120" windowHeight="16060" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="51200" windowHeight="28340" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Metadata" sheetId="9" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="247" uniqueCount="186">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="245" uniqueCount="184">
   <si>
     <t>organisation_path</t>
   </si>
@@ -567,12 +567,6 @@
   </si>
   <si>
     <t>organisation_end_date</t>
-  </si>
-  <si>
-    <t>organisation_omsss_email</t>
-  </si>
-  <si>
-    <t>org1@mail.example.com</t>
   </si>
   <si>
     <t>key</t>
@@ -646,26 +640,23 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="6">
+  <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="5" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="6">
+  <cellStyles count="5">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="5" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -968,7 +959,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DC210344-960F-5D41-9375-863DD1899BAF}">
   <dimension ref="A1:B3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
@@ -976,23 +967,23 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="B1" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="B2" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="B3">
         <v>2</v>
@@ -1164,7 +1155,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:AC5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="AC5" sqref="AC5"/>
     </sheetView>
   </sheetViews>
@@ -1253,7 +1244,7 @@
         <v>43</v>
       </c>
       <c r="AB1" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="AC1" t="s">
         <v>44</v>
@@ -2272,9 +2263,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:BD3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
@@ -2794,7 +2783,7 @@
         <v>3</v>
       </c>
       <c r="BB3">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="BC3">
         <v>5</v>
@@ -2950,11 +2939,9 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
-  <dimension ref="A1:K2"/>
+  <dimension ref="A1:J2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I4" sqref="I4"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
@@ -2963,10 +2950,10 @@
     <col min="3" max="3" width="25.6640625" customWidth="1"/>
     <col min="4" max="4" width="21.6640625" customWidth="1"/>
     <col min="5" max="5" width="20.5" customWidth="1"/>
-    <col min="8" max="10" width="10.83203125" style="2"/>
+    <col min="8" max="9" width="10.83203125" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2994,14 +2981,11 @@
       <c r="I1" s="2" t="s">
         <v>177</v>
       </c>
-      <c r="J1" s="2" t="s">
-        <v>178</v>
-      </c>
-      <c r="K1" t="s">
+      <c r="J1" t="s">
         <v>172</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>11</v>
       </c>
@@ -3023,14 +3007,8 @@
       <c r="H2" s="2" t="s">
         <v>176</v>
       </c>
-      <c r="J2" s="3" t="s">
-        <v>179</v>
-      </c>
     </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="J2" r:id="rId1" xr:uid="{7B3AA911-53A5-3445-88E8-2DB7B9629137}"/>
-  </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">

</xml_diff>

<commit_message>
Fixup org data range to pass validations
</commit_message>
<xml_diff>
--- a/data/_orig/pmhc-upload.xlsx
+++ b/data/_orig/pmhc-upload.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/russellj/stratdat/pmhc/spec/data/_orig/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF7E0106-773B-EB4D-B0A3-367B96F308D7}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5837FB5A-3B28-6C46-BE55-CE1DE1266331}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="51200" windowHeight="28340" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="51200" windowHeight="28340" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Metadata" sheetId="9" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="245" uniqueCount="184">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="246" uniqueCount="185">
   <si>
     <t>organisation_path</t>
   </si>
@@ -563,9 +563,6 @@
     <t>organisation_start_date</t>
   </si>
   <si>
-    <t>01072016</t>
-  </si>
-  <si>
     <t>organisation_end_date</t>
   </si>
   <si>
@@ -585,6 +582,12 @@
   </si>
   <si>
     <t>continuity_of_support</t>
+  </si>
+  <si>
+    <t>01072014</t>
+  </si>
+  <si>
+    <t>09099999</t>
   </si>
 </sst>
 </file>
@@ -959,31 +962,31 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DC210344-960F-5D41-9375-863DD1899BAF}">
   <dimension ref="A1:B3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="AE22" sqref="AE22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
+        <v>177</v>
+      </c>
+      <c r="B1" t="s">
         <v>178</v>
-      </c>
-      <c r="B1" t="s">
-        <v>179</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
+        <v>179</v>
+      </c>
+      <c r="B2" t="s">
         <v>180</v>
-      </c>
-      <c r="B2" t="s">
-        <v>181</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="B3">
         <v>2</v>
@@ -1244,7 +1247,7 @@
         <v>43</v>
       </c>
       <c r="AB1" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="AC1" t="s">
         <v>44</v>
@@ -2941,7 +2944,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:J2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I2" sqref="I2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
@@ -2979,7 +2984,7 @@
         <v>175</v>
       </c>
       <c r="I1" s="2" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="J1" t="s">
         <v>172</v>
@@ -3005,7 +3010,10 @@
         <v>1</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>176</v>
+        <v>183</v>
+      </c>
+      <c r="I2" s="2" t="s">
+        <v>184</v>
       </c>
     </row>
   </sheetData>

</xml_diff>